<commit_message>
remove Excel formulas. Everything happens in Java
</commit_message>
<xml_diff>
--- a/src/main/resources/template/Anschreiben_Vorlage.xlsx
+++ b/src/main/resources/template/Anschreiben_Vorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\IdeaProjects\rent-index\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C8CD3C-A515-4E56-958C-E36582DD1A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A472243-23CD-4D76-AB01-EEB53F6CC7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1030" yWindow="1720" windowWidth="19190" windowHeight="10190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seite1" sheetId="1" r:id="rId1"/>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1507"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -878,7 +878,7 @@
       </c>
       <c r="H14" s="13">
         <f ca="1">TODAY()</f>
-        <v>45847</v>
+        <v>45848</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
@@ -1094,14 +1094,12 @@
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="28">
-        <f>G30</f>
-        <v>118.2</v>
+        <v>118</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="33">
-        <f>G27</f>
         <v>102.7</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -1109,7 +1107,7 @@
       </c>
       <c r="E36" s="35">
         <f>A36/C36*100-100</f>
-        <v>15.092502434274579</v>
+        <v>14.897760467380721</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>12</v>
@@ -1136,7 +1134,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="24"/>
       <c r="H39" s="29">
-        <v>1605</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1155,23 +1153,20 @@
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="34">
-        <f>E36</f>
-        <v>15.092502434274579</v>
+        <v>4.01</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="32">
-        <f>H41-H39</f>
-        <v>242</v>
+        <v>111</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H41" s="25">
-        <f>ROUNDDOWN(G30/G27*H39, 0)</f>
-        <v>1847</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1208,7 +1203,7 @@
       <c r="F44" s="4"/>
       <c r="H44" s="27">
         <f>H41+H42</f>
-        <v>1957</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="2" customFormat="1" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">

</xml_diff>